<commit_message>
Solved save and reload bug
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -1,253 +1,262 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="76">
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optimizer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uniform sampler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loss function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lr_init</t>
-  </si>
-  <si>
-    <t xml:space="preserve">momentum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lr scheduler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lr decay period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pretrained</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of iter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loss_tr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loss_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCR1_tr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCR1_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August28  18:58:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27_07_17_mit_indoor/resnet50_mit_indoor_sgd_crossentropy_July26  10:31:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">synthetic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sgd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multisoft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7fdcd1c628c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tested for Brians BR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August28  21:42:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f7d4c623950&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tested for Rural LR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August28  23:46:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7fe7443b48c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  11:01:57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7fb8699908c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tested for three rooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  11:48:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f0f2c01a8c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tested for BR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  12:26:32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loaded_synthetic_sgd_multisoft_August29  11:48:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f0f2c01a840&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  12:30:42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f0f2c01a7b8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  12:32:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f458abcb840&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  12:52:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f6d72d868c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  14:35:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7fc56cf76950&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  15:40:41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resnet50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7fcd7e4ac8c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  16:27:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7fa5c080a8c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  18:30:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resnet18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">real</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f16c510f8c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  18:46:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7fdf1fd9b8c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  19:06:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f19dfb7a8c8&gt;</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>Uniform sampler</t>
+  </si>
+  <si>
+    <t>Loss function</t>
+  </si>
+  <si>
+    <t>lr_init</t>
+  </si>
+  <si>
+    <t>momentum</t>
+  </si>
+  <si>
+    <t>lr scheduler</t>
+  </si>
+  <si>
+    <t>lr decay period</t>
+  </si>
+  <si>
+    <t>pretrained</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>Number of iter</t>
+  </si>
+  <si>
+    <t>loss_tr</t>
+  </si>
+  <si>
+    <t>loss_test</t>
+  </si>
+  <si>
+    <t>CCR1_tr</t>
+  </si>
+  <si>
+    <t>CCR1_test</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>August28  18:58:36</t>
+  </si>
+  <si>
+    <t>27_07_17_mit_indoor/resnet50_mit_indoor_sgd_crossentropy_July26  10:31:05</t>
+  </si>
+  <si>
+    <t>synthetic</t>
+  </si>
+  <si>
+    <t>sgd</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>multisoft</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fdcd1c628c8&gt;</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Tested for Brians BR</t>
+  </si>
+  <si>
+    <t>August28  21:42:06</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f7d4c623950&gt;</t>
+  </si>
+  <si>
+    <t>Tested for Rural LR</t>
+  </si>
+  <si>
+    <t>August28  23:46:14</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fe7443b48c8&gt;</t>
+  </si>
+  <si>
+    <t>August29  11:01:57</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fb8699908c8&gt;</t>
+  </si>
+  <si>
+    <t>Tested for three rooms</t>
+  </si>
+  <si>
+    <t>August29  11:48:59</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f0f2c01a8c8&gt;</t>
+  </si>
+  <si>
+    <t>Tested for BR</t>
+  </si>
+  <si>
+    <t>August29  12:26:32</t>
+  </si>
+  <si>
+    <t>loaded_synthetic_sgd_multisoft_August29  11:48:59</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f0f2c01a840&gt;</t>
+  </si>
+  <si>
+    <t>August29  12:30:42</t>
+  </si>
+  <si>
+    <t>0.0005</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f0f2c01a7b8&gt;</t>
+  </si>
+  <si>
+    <t>August29  12:32:04</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f458abcb840&gt;</t>
+  </si>
+  <si>
+    <t>August29  12:52:13</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f6d72d868c8&gt;</t>
+  </si>
+  <si>
+    <t>August29  14:35:30</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fc56cf76950&gt;</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>August29  15:40:41</t>
+  </si>
+  <si>
+    <t>resnet50</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fcd7e4ac8c8&gt;</t>
+  </si>
+  <si>
+    <t>August29  16:27:20</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fa5c080a8c8&gt;</t>
+  </si>
+  <si>
+    <t>August29  18:30:10</t>
+  </si>
+  <si>
+    <t>resnet18</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f16c510f8c8&gt;</t>
+  </si>
+  <si>
+    <t>August29  18:46:14</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fdf1fd9b8c8&gt;</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>August29  19:06:27</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f19dfb7a8c8&gt;</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">August29  19:42:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f19dfb7a840&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August29  20:20:52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f19dfb7a7b8&gt;</t>
+    <t>August29  19:42:44</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f19dfb7a840&gt;</t>
+  </si>
+  <si>
+    <t>August29  20:20:52</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f19dfb7a7b8&gt;</t>
+  </si>
+  <si>
+    <t>August30  15:09:39</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fad0bb60950&gt;</t>
+  </si>
+  <si>
+    <t>August30  15:10:05</t>
+  </si>
+  <si>
+    <t>August30  15:10:20</t>
   </si>
 </sst>
 </file>
@@ -255,48 +264,48 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt formatCode="General" numFmtId="164"/>
   </numFmts>
   <fonts count="5">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -304,84 +313,350 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="4">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="R19" activeCellId="0" pane="topLeft" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.25"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.77551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.02040816326531"/>
+    <col customWidth="1" max="1" min="1" style="1" width="21.6683673469388"/>
+    <col customWidth="1" max="2" min="2" style="1" width="17.0918367346939"/>
+    <col customWidth="1" max="3" min="3" style="1" width="11.25"/>
+    <col customWidth="1" max="4" min="4" style="1" width="10.969387755102"/>
+    <col customWidth="1" max="5" min="5" style="1" width="15.1377551020408"/>
+    <col customWidth="1" max="6" min="6" style="1" width="10.6938775510204"/>
+    <col customWidth="1" max="7" min="7" style="1" width="8.77551020408163"/>
+    <col customWidth="1" max="8" min="8" style="1" width="8.23469387755102"/>
+    <col customWidth="1" max="9" min="9" style="1" width="12.0867346938776"/>
+    <col customWidth="1" max="10" min="10" style="1" width="7.77551020408163"/>
+    <col customWidth="1" max="11" min="11" style="1" width="9.045918367346941"/>
+    <col customWidth="1" max="1025" min="12" style="1" width="7.02040816326531"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="13.8" r="1" s="3" spans="1:18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -437,7 +712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="2" s="3" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -493,7 +768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="3" s="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -549,7 +824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="4" s="3" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -605,7 +880,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="5" s="3" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -661,7 +936,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="6" s="3" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -717,7 +992,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="7" s="3" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -767,13 +1042,13 @@
         <v>0.825</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>0.853333333333333</v>
+        <v>0.8533333333333331</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="8" s="3" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -810,16 +1085,16 @@
       <c r="L8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="0"/>
-      <c r="N8" s="0"/>
-      <c r="O8" s="0"/>
-      <c r="P8" s="0"/>
-      <c r="Q8" s="0"/>
+      <c r="M8" s="1" t="n"/>
+      <c r="N8" s="1" t="n"/>
+      <c r="O8" s="1" t="n"/>
+      <c r="P8" s="1" t="n"/>
+      <c r="Q8" s="1" t="n"/>
       <c r="R8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="9" s="3" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -875,7 +1150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="10" s="3" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -931,7 +1206,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="11" s="3" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -987,7 +1262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="12" s="3" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1043,7 +1318,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="13" s="3" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -1099,7 +1374,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="14" s="3" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -1152,7 +1427,7 @@
         <v>0.556231003039514</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="15" s="3" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1205,7 +1480,7 @@
         <v>0.814589665653495</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="16" s="3" spans="1:18">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -1261,7 +1536,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="17" s="3" spans="1:18">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -1317,7 +1592,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="15" r="18" s="3" spans="1:18">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -1373,13 +1648,162 @@
         <v>71</v>
       </c>
     </row>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.03335192694794387</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.02937221649388774</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.6028645833333334</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.6717325227963525</v>
+      </c>
+      <c r="R19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s">
+        <v>68</v>
+      </c>
+      <c r="R20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" t="n">
+        <v>4</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.01419249125562298</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.02507951604287313</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.94921875</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.8389057750759878</v>
+      </c>
+      <c r="R21" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>